<commit_message>
Tried new logic for material demand
</commit_message>
<xml_diff>
--- a/data/raw_data/V2G_scenarios.xlsx
+++ b/data/raw_data/V2G_scenarios.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10215"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauinger\Desktop\dirk\Second-Life Batteries\code_git\V2G_in_EU\data\raw_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernaag/Library/CloudStorage/Box-Box/BATMAN/Coding/V2G_in_EU/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9CA9927-1771-1840-9D5E-C7073D9043C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5175" yWindow="3000" windowWidth="28035" windowHeight="17445"/>
+    <workbookView xWindow="5300" yWindow="3220" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -402,16 +403,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -425,9 +426,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -439,9 +440,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -450,12 +451,12 @@
         <v>2030</v>
       </c>
       <c r="D3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -464,12 +465,12 @@
         <v>2050</v>
       </c>
       <c r="D4">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -481,9 +482,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -492,12 +493,12 @@
         <v>2030</v>
       </c>
       <c r="D6">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
@@ -506,12 +507,12 @@
         <v>2050</v>
       </c>
       <c r="D7">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
@@ -523,9 +524,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
         <v>4</v>
@@ -534,12 +535,12 @@
         <v>2030</v>
       </c>
       <c r="D9">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
         <v>4</v>
@@ -548,12 +549,12 @@
         <v>2050</v>
       </c>
       <c r="D10">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
@@ -565,35 +566,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
       </c>
       <c r="C12">
-        <v>2028</v>
+        <v>2030</v>
       </c>
       <c r="D12">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
         <v>4</v>
       </c>
       <c r="C13">
-        <v>2031</v>
+        <v>2050</v>
       </c>
       <c r="D13">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -601,13 +602,13 @@
         <v>4</v>
       </c>
       <c r="C14">
-        <v>2035</v>
+        <v>2020</v>
       </c>
       <c r="D14">
-        <v>0.88</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -615,43 +616,43 @@
         <v>4</v>
       </c>
       <c r="C15">
-        <v>2050</v>
+        <v>2028</v>
       </c>
       <c r="D15">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16" t="s">
         <v>4</v>
       </c>
       <c r="C16">
-        <v>2020</v>
+        <v>2031</v>
       </c>
       <c r="D16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s">
         <v>4</v>
       </c>
       <c r="C17">
-        <v>2030</v>
+        <v>2035</v>
       </c>
       <c r="D17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B18" t="s">
         <v>4</v>
@@ -660,10 +661,10 @@
         <v>2050</v>
       </c>
       <c r="D18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -677,7 +678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -691,7 +692,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -705,7 +706,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -719,7 +720,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>10</v>
       </c>

</xml_diff>